<commit_message>
Updating login test cases
Added successful logout test case
</commit_message>
<xml_diff>
--- a/manual-testing/test-cases/Login_Test_Cases.xlsx
+++ b/manual-testing/test-cases/Login_Test_Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -101,6 +101,25 @@
   <si>
     <t>username: abcdef
 password: secret_sauce</t>
+  </si>
+  <si>
+    <t>TC_LOGOUT_01</t>
+  </si>
+  <si>
+    <t>Logout successfully</t>
+  </si>
+  <si>
+    <t>User is logged in and on the Products page</t>
+  </si>
+  <si>
+    <t>1. Click side menu on the bottom left
+2. Click the logout button</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>User is logged out and gets redirected to login page</t>
   </si>
 </sst>
 </file>
@@ -399,6 +418,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="14.88"/>
     <col customWidth="1" min="2" max="2" width="22.0"/>
     <col customWidth="1" min="3" max="3" width="20.13"/>
     <col customWidth="1" min="4" max="4" width="25.88"/>
@@ -543,15 +563,31 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="6"/>
+      <c r="H6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4"/>
@@ -10505,10 +10541,10 @@
     </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H6">
       <formula1>"Low,Medium,High"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I5">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="I2:I6">
       <formula1>"Not Run,Pass,Fail,In Progress,Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>